<commit_message>
added s2p folder migration and fixed xlsx column names
</commit_message>
<xml_diff>
--- a/oldnames_to_new.xlsx
+++ b/oldnames_to_new.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27932"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matilde.perrino\code\neuro-group-jfish\src\temporary\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matilde/code/calcium-imaging-pipeline/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32C25BD2-90C8-4516-909E-B05835615F59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A23AC011-7997-D849-97B8-522D384E849B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="780" windowWidth="18960" windowHeight="13440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,9 +20,6 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
-      <xlwcv:version setVersion="1"/>
-    </ext>
   </extLst>
 </workbook>
 </file>
@@ -39,12 +36,6 @@
     <t>experimenter</t>
   </si>
   <si>
-    <t>fish_id_old</t>
-  </si>
-  <si>
-    <t>fish_id</t>
-  </si>
-  <si>
     <t>LR_bout_continous</t>
   </si>
   <si>
@@ -349,6 +340,12 @@
   </si>
   <si>
     <t>speed_groupsize_thalamus_exp03</t>
+  </si>
+  <si>
+    <t>old_name</t>
+  </si>
+  <si>
+    <t>new_name</t>
   </si>
 </sst>
 </file>
@@ -707,21 +704,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
-      <selection activeCell="I75" sqref="I75"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="27.42578125" customWidth="1"/>
+    <col min="1" max="2" width="27.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>1</v>
@@ -730,1530 +727,1530 @@
         <v>2</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>3</v>
+        <v>105</v>
       </c>
       <c r="F1" s="4" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>6</v>
-      </c>
       <c r="D2" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E2" s="1">
         <v>1</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E3" s="1">
         <v>2</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E4" s="1">
         <v>3</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E5" s="1">
         <v>4</v>
       </c>
       <c r="F5" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" s="1">
+        <v>5</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6" s="1">
-        <v>5</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="D7" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E7" s="1">
         <v>6</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E8" s="1">
         <v>7</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E9" s="1">
         <v>8</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E10" s="1">
         <v>9</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E11" s="1">
         <v>10</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E12" s="1">
         <v>11</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E13" s="1">
         <v>12</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E14" s="1">
         <v>13</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E15" s="1">
         <v>14</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E16" s="1">
         <v>15</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E17" s="1">
         <v>16</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E18" s="1">
         <v>17</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E19" s="1">
         <v>18</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E20" s="1">
         <v>19</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E21" s="1">
         <v>20</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E22" s="1">
         <v>21</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E23" s="1">
         <v>22</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E24" s="1">
         <v>23</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E25" s="1">
         <v>24</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E26" s="1">
         <v>25</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E27" s="1">
         <v>26</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E28" s="1">
         <v>27</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E29" s="1">
         <v>28</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E30" s="1">
         <v>29</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E31" s="1">
         <v>30</v>
       </c>
       <c r="F31" s="5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E32" s="1">
         <v>31</v>
       </c>
       <c r="F32" s="5" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E33" s="1">
         <v>32</v>
       </c>
       <c r="F33" s="5" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E34" s="1">
         <v>33</v>
       </c>
       <c r="F34" s="5" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E35" s="1">
         <v>34</v>
       </c>
       <c r="F35" s="5" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E36" s="1">
         <v>35</v>
       </c>
       <c r="F36" s="5" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E37" s="1">
         <v>36</v>
       </c>
       <c r="F37" s="5" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E38" s="1">
         <v>37</v>
       </c>
       <c r="F38" s="5" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E39" s="1">
         <v>38</v>
       </c>
       <c r="F39" s="5" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E40" s="1">
         <v>39</v>
       </c>
       <c r="F40" s="5" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E41" s="1">
         <v>40</v>
       </c>
       <c r="F41" s="5" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E42" s="1">
         <v>41</v>
       </c>
       <c r="F42" s="5" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E43" s="1">
         <v>42</v>
       </c>
       <c r="F43" s="5" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E44" s="1">
         <v>43</v>
       </c>
       <c r="F44" s="5" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E45" s="1">
         <v>1</v>
       </c>
       <c r="F45" s="5" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E46" s="1">
         <v>2</v>
       </c>
       <c r="F46" s="5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A47" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E47" s="1">
+        <v>3</v>
+      </c>
+      <c r="F47" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A48" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C48" s="3" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="47" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A47" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="C47" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D47" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E47" s="1">
-        <v>3</v>
-      </c>
-      <c r="F47" s="5" t="s">
+      <c r="D48" s="1" t="s">
         <v>65</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A48" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="C48" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="D48" s="1" t="s">
-        <v>67</v>
       </c>
       <c r="E48" s="1">
         <v>4</v>
       </c>
       <c r="F48" s="5" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D49" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E49" s="1">
+        <v>5</v>
+      </c>
+      <c r="F49" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="E49" s="1">
-        <v>5</v>
-      </c>
-      <c r="F49" s="5" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="50" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E50" s="1">
         <v>6</v>
       </c>
       <c r="F50" s="5" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E51" s="1">
         <v>7</v>
       </c>
       <c r="F51" s="5" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E52" s="1">
         <v>8</v>
       </c>
       <c r="F52" s="5" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E53" s="1">
         <v>9</v>
       </c>
       <c r="F53" s="5" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E54" s="1">
         <v>10</v>
       </c>
       <c r="F54" s="5" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E55" s="1">
         <v>11</v>
       </c>
       <c r="F55" s="5" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E56" s="1">
         <v>12</v>
       </c>
       <c r="F56" s="5" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E57" s="1">
         <v>13</v>
       </c>
       <c r="F57" s="5" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E58" s="1">
         <v>14</v>
       </c>
       <c r="F58" s="5" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E59" s="1">
         <v>1</v>
       </c>
       <c r="F59" s="5" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E60" s="1">
         <v>2</v>
       </c>
       <c r="F60" s="5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A61" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C61" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E61" s="1">
+        <v>3</v>
+      </c>
+      <c r="F61" s="6" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="61" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A61" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="B61" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="C61" s="3" t="s">
+    <row r="62" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A62" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C62" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D62" s="1" t="s">
         <v>83</v>
-      </c>
-      <c r="D61" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E61" s="1">
-        <v>3</v>
-      </c>
-      <c r="F61" s="6" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A62" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="B62" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="C62" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="D62" s="1" t="s">
-        <v>85</v>
       </c>
       <c r="E62" s="1">
         <v>4</v>
       </c>
       <c r="F62" s="6" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C63" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D63" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="D63" s="1" t="s">
+      <c r="E63" s="1">
+        <v>5</v>
+      </c>
+      <c r="F63" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="E63" s="1">
-        <v>5</v>
-      </c>
-      <c r="F63" s="6" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="64" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C64" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D64" s="1" t="s">
         <v>83</v>
-      </c>
-      <c r="D64" s="1" t="s">
-        <v>85</v>
       </c>
       <c r="E64" s="1">
         <v>6</v>
       </c>
       <c r="F64" s="6" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C65" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D65" s="1" t="s">
         <v>83</v>
-      </c>
-      <c r="D65" s="1" t="s">
-        <v>85</v>
       </c>
       <c r="E65" s="1">
         <v>7</v>
       </c>
       <c r="F65" s="6" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C66" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D66" s="1" t="s">
         <v>83</v>
-      </c>
-      <c r="D66" s="1" t="s">
-        <v>85</v>
       </c>
       <c r="E66" s="1">
         <v>8</v>
       </c>
       <c r="F66" s="6" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C67" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D67" s="1" t="s">
         <v>83</v>
-      </c>
-      <c r="D67" s="1" t="s">
-        <v>85</v>
       </c>
       <c r="E67" s="1">
         <v>9</v>
       </c>
       <c r="F67" s="6" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E68" s="1">
         <v>10</v>
       </c>
       <c r="F68" s="5" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E69" s="1">
         <v>11</v>
       </c>
       <c r="F69" s="5" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E70" s="1">
         <v>12</v>
       </c>
       <c r="F70" s="5" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E71" s="1">
         <v>13</v>
       </c>
       <c r="F71" s="5" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E72" s="1">
         <v>14</v>
       </c>
       <c r="F72" s="5" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E73" s="1">
         <v>15</v>
       </c>
       <c r="F73" s="5" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E74" s="1">
         <v>16</v>
       </c>
       <c r="F74" s="5" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E75" s="1">
         <v>17</v>
       </c>
       <c r="F75" s="5" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E76" s="1">
         <v>15</v>
       </c>
       <c r="F76" s="5" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E77" s="1">
         <v>44</v>
       </c>
       <c r="F77" s="5" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>